<commit_message>
[fix] Corrected number of pages on tags
</commit_message>
<xml_diff>
--- a/tags.xlsx
+++ b/tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\npl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9EDF88-D4DD-43CA-881D-59C286763C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174C4308-1ACC-4834-AC9B-884CBAE9E1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BB445A06-7D9C-4119-A89F-F95577B246BF}"/>
   </bookViews>
@@ -18,19 +18,12 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">graphs!$G$210:$K$372</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tags!$A$1:$E$183</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">graphs!$U$2:$U$183</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">graphs!$V$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">graphs!$J$211:$J$372</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">graphs!$K$211:$K$372</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">graphs!$V$2:$V$183</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">graphs!$U$2:$U$183</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">graphs!$V$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">graphs!$V$2:$V$183</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">graphs!$J$211:$J$372</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">graphs!$K$211:$K$372</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">graphs!$J$211:$J$372</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">graphs!$K$211:$K$372</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tags!$A$1:$F$183</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">graphs!$J$211:$J$372</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">graphs!$K$211:$K$372</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">graphs!$U$2:$U$183</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">graphs!$V$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">graphs!$V$2:$V$183</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -926,6 +919,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-EE44-4CCE-AFC8-C8D507C52FCD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -941,6 +939,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-EE44-4CCE-AFC8-C8D507C52FCD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -956,6 +959,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-EE44-4CCE-AFC8-C8D507C52FCD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -971,6 +979,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-EE44-4CCE-AFC8-C8D507C52FCD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -986,6 +999,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-EE44-4CCE-AFC8-C8D507C52FCD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -1113,6 +1131,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-EE44-4CCE-AFC8-C8D507C52FCD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -1499,10 +1522,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1540,7 +1563,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{137DB9EA-BE46-4AE5-A3A7-0F85F2BC2514}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>Error</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1583,10 +1606,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3802,7 +3825,7 @@
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3966,9 +3989,6 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>8</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -3987,7 +4007,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -4007,7 +4027,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -4027,7 +4047,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -4047,7 +4067,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -4066,9 +4086,6 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13">
-        <v>80</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -4087,7 +4104,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -4107,7 +4124,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>24</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -4127,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>92</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -4147,7 +4164,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>104</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -4167,7 +4184,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>22</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -4186,9 +4203,6 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19">
-        <v>86</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
@@ -4206,9 +4220,6 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20">
-        <v>72</v>
-      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
@@ -4227,7 +4238,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -4247,7 +4258,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>116</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -4267,7 +4278,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -4287,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -4307,7 +4318,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>64</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -4327,7 +4338,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -4347,7 +4358,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -4367,7 +4378,7 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -4387,7 +4398,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -4407,7 +4418,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>24</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -4427,7 +4438,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>68</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -4447,7 +4458,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>56</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -4487,7 +4498,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>100</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -4507,7 +4518,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -4527,7 +4538,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -4547,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -4567,7 +4578,7 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>139</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -4587,7 +4598,7 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>268</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -4607,7 +4618,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -4627,7 +4638,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -4647,7 +4658,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>68</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -4667,7 +4678,7 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>19</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -4687,7 +4698,7 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -4707,7 +4718,7 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -4727,7 +4738,7 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -4747,7 +4758,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>48</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -4767,7 +4778,7 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -4787,7 +4798,7 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>181</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -4806,9 +4817,6 @@
       <c r="E50">
         <v>1</v>
       </c>
-      <c r="F50">
-        <v>96</v>
-      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
@@ -4827,7 +4835,7 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>160</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -4847,7 +4855,7 @@
         <v>0</v>
       </c>
       <c r="F52">
-        <v>104</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -4867,7 +4875,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>120</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -4887,7 +4895,7 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>136</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -4907,7 +4915,7 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <v>64</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -4927,7 +4935,7 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <v>84</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -4947,7 +4955,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>124</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -4967,7 +4975,7 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <v>23</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -4987,7 +4995,7 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>36</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -5006,9 +5014,6 @@
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="F60">
-        <v>32</v>
-      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
@@ -5027,7 +5032,7 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>156</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -5047,7 +5052,7 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <v>108</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -5067,7 +5072,7 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>28</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -5087,7 +5092,7 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <v>108</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -5107,7 +5112,7 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <v>92</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -5126,9 +5131,6 @@
       <c r="E66">
         <v>1</v>
       </c>
-      <c r="F66">
-        <v>116</v>
-      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
@@ -5147,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
@@ -5167,7 +5169,7 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <v>44</v>
+        <v>156</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -5187,7 +5189,7 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <v>56</v>
+        <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -5207,7 +5209,7 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
@@ -5227,7 +5229,7 @@
         <v>0</v>
       </c>
       <c r="F71">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -5247,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="F72">
-        <v>52</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -5267,7 +5269,7 @@
         <v>0</v>
       </c>
       <c r="F73">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -5287,7 +5289,7 @@
         <v>0</v>
       </c>
       <c r="F74">
-        <v>228</v>
+        <v>48</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -5307,7 +5309,7 @@
         <v>0</v>
       </c>
       <c r="F75">
-        <v>132</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
@@ -5327,7 +5329,7 @@
         <v>0</v>
       </c>
       <c r="F76">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
@@ -5347,7 +5349,7 @@
         <v>0</v>
       </c>
       <c r="F77">
-        <v>108</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
@@ -5367,7 +5369,7 @@
         <v>0</v>
       </c>
       <c r="F78">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -5407,7 +5409,7 @@
         <v>0</v>
       </c>
       <c r="F80">
-        <v>64</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
@@ -5427,7 +5429,7 @@
         <v>0</v>
       </c>
       <c r="F81">
-        <v>116</v>
+        <v>228</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
@@ -5447,7 +5449,7 @@
         <v>0</v>
       </c>
       <c r="F82">
-        <v>80</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
@@ -5467,7 +5469,7 @@
         <v>0</v>
       </c>
       <c r="F83">
-        <v>44</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
@@ -5487,7 +5489,7 @@
         <v>0</v>
       </c>
       <c r="F84">
-        <v>80</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
@@ -5507,7 +5509,7 @@
         <v>0</v>
       </c>
       <c r="F85">
-        <v>148</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
@@ -5527,7 +5529,7 @@
         <v>0</v>
       </c>
       <c r="F86">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
@@ -5547,7 +5549,7 @@
         <v>0</v>
       </c>
       <c r="F87">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
@@ -5566,9 +5568,6 @@
       <c r="E88">
         <v>1</v>
       </c>
-      <c r="F88">
-        <v>92</v>
-      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
@@ -5587,7 +5586,7 @@
         <v>0</v>
       </c>
       <c r="F89">
-        <v>72</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
@@ -5607,7 +5606,7 @@
         <v>0</v>
       </c>
       <c r="F90">
-        <v>120</v>
+        <v>80</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -5627,7 +5626,7 @@
         <v>0</v>
       </c>
       <c r="F91">
-        <v>100</v>
+        <v>44</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
@@ -5647,7 +5646,7 @@
         <v>0</v>
       </c>
       <c r="F92">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -5667,7 +5666,7 @@
         <v>0</v>
       </c>
       <c r="F93">
-        <v>76</v>
+        <v>148</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -5687,7 +5686,7 @@
         <v>0</v>
       </c>
       <c r="F94">
-        <v>92</v>
+        <v>56</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
@@ -5707,7 +5706,7 @@
         <v>0</v>
       </c>
       <c r="F95">
-        <v>54</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
@@ -5727,7 +5726,7 @@
         <v>0</v>
       </c>
       <c r="F96">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -5746,9 +5745,6 @@
       <c r="E97">
         <v>1</v>
       </c>
-      <c r="F97">
-        <v>76</v>
-      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98">
@@ -5767,7 +5763,7 @@
         <v>0</v>
       </c>
       <c r="F98">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -5787,7 +5783,7 @@
         <v>0</v>
       </c>
       <c r="F99">
-        <v>64</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
@@ -5807,7 +5803,7 @@
         <v>0</v>
       </c>
       <c r="F100">
-        <v>52</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
@@ -5827,7 +5823,7 @@
         <v>0</v>
       </c>
       <c r="F101">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -5847,7 +5843,7 @@
         <v>0</v>
       </c>
       <c r="F102">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -5867,7 +5863,7 @@
         <v>0</v>
       </c>
       <c r="F103">
-        <v>33</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -5887,7 +5883,7 @@
         <v>0</v>
       </c>
       <c r="F104">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
@@ -5907,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="F105">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
@@ -5927,7 +5923,7 @@
         <v>0</v>
       </c>
       <c r="F106">
-        <v>136</v>
+        <v>76</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
@@ -5947,7 +5943,7 @@
         <v>0</v>
       </c>
       <c r="F107">
-        <v>64</v>
+        <v>92</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
@@ -5967,7 +5963,7 @@
         <v>0</v>
       </c>
       <c r="F108">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
@@ -5987,7 +5983,7 @@
         <v>0</v>
       </c>
       <c r="F109">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
@@ -6007,7 +6003,7 @@
         <v>0</v>
       </c>
       <c r="F110">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
@@ -6026,9 +6022,6 @@
       <c r="E111">
         <v>1</v>
       </c>
-      <c r="F111">
-        <v>28</v>
-      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112">
@@ -6046,9 +6039,6 @@
       <c r="E112">
         <v>1</v>
       </c>
-      <c r="F112">
-        <v>108</v>
-      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113">
@@ -6067,7 +6057,7 @@
         <v>0</v>
       </c>
       <c r="F113">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
@@ -6087,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="F114">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
@@ -6106,9 +6096,6 @@
       <c r="E115">
         <v>1</v>
       </c>
-      <c r="F115">
-        <v>56</v>
-      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116">
@@ -6127,7 +6114,7 @@
         <v>0</v>
       </c>
       <c r="F116">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
@@ -6147,7 +6134,7 @@
         <v>0</v>
       </c>
       <c r="F117">
-        <v>20</v>
+        <v>96</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
@@ -6167,7 +6154,7 @@
         <v>0</v>
       </c>
       <c r="F118">
-        <v>48</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
@@ -6207,7 +6194,7 @@
         <v>0</v>
       </c>
       <c r="F120">
-        <v>11</v>
+        <v>80</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
@@ -6227,7 +6214,7 @@
         <v>0</v>
       </c>
       <c r="F121">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
@@ -6247,7 +6234,7 @@
         <v>0</v>
       </c>
       <c r="F122">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
@@ -6267,7 +6254,7 @@
         <v>0</v>
       </c>
       <c r="F123">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
@@ -6287,7 +6274,7 @@
         <v>0</v>
       </c>
       <c r="F124">
-        <v>64</v>
+        <v>108</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
@@ -6307,7 +6294,7 @@
         <v>0</v>
       </c>
       <c r="F125">
-        <v>16</v>
+        <v>82</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
@@ -6327,7 +6314,7 @@
         <v>0</v>
       </c>
       <c r="F126">
-        <v>68</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
@@ -6347,7 +6334,7 @@
         <v>0</v>
       </c>
       <c r="F127">
-        <v>108</v>
+        <v>56</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
@@ -6367,7 +6354,7 @@
         <v>0</v>
       </c>
       <c r="F128">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
@@ -6387,7 +6374,7 @@
         <v>0</v>
       </c>
       <c r="F129">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
@@ -6407,7 +6394,7 @@
         <v>0</v>
       </c>
       <c r="F130">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
@@ -6427,7 +6414,7 @@
         <v>0</v>
       </c>
       <c r="F131">
-        <v>116</v>
+        <v>64</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.35">
@@ -6447,7 +6434,7 @@
         <v>0</v>
       </c>
       <c r="F132">
-        <v>80</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
@@ -6467,7 +6454,7 @@
         <v>0</v>
       </c>
       <c r="F133">
-        <v>92</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
@@ -6487,7 +6474,7 @@
         <v>0</v>
       </c>
       <c r="F134">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
@@ -6507,7 +6494,7 @@
         <v>0</v>
       </c>
       <c r="F135">
-        <v>58</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
@@ -6527,7 +6514,7 @@
         <v>0</v>
       </c>
       <c r="F136">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
@@ -6547,7 +6534,7 @@
         <v>0</v>
       </c>
       <c r="F137">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
@@ -6567,7 +6554,7 @@
         <v>0</v>
       </c>
       <c r="F138">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
@@ -6586,9 +6573,6 @@
       <c r="E139">
         <v>1</v>
       </c>
-      <c r="F139">
-        <v>52</v>
-      </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140">
@@ -6607,7 +6591,7 @@
         <v>0</v>
       </c>
       <c r="F140">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.35">
@@ -6627,7 +6611,7 @@
         <v>0</v>
       </c>
       <c r="F141">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.35">
@@ -6647,7 +6631,7 @@
         <v>0</v>
       </c>
       <c r="F142">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
@@ -6667,7 +6651,7 @@
         <v>0</v>
       </c>
       <c r="F143">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
@@ -6687,7 +6671,7 @@
         <v>0</v>
       </c>
       <c r="F144">
-        <v>68</v>
+        <v>116</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.35">
@@ -6707,7 +6691,7 @@
         <v>0</v>
       </c>
       <c r="F145">
-        <v>52</v>
+        <v>80</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.35">
@@ -6727,7 +6711,7 @@
         <v>0</v>
       </c>
       <c r="F146">
-        <v>16</v>
+        <v>92</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.35">
@@ -6747,7 +6731,7 @@
         <v>0</v>
       </c>
       <c r="F147">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
@@ -6767,7 +6751,7 @@
         <v>0</v>
       </c>
       <c r="F148">
-        <v>8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
@@ -6787,7 +6771,7 @@
         <v>0</v>
       </c>
       <c r="F149">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.35">
@@ -6807,7 +6791,7 @@
         <v>0</v>
       </c>
       <c r="F150">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
@@ -6827,7 +6811,7 @@
         <v>0</v>
       </c>
       <c r="F151">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.35">
@@ -6847,7 +6831,7 @@
         <v>0</v>
       </c>
       <c r="F152">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.35">
@@ -6867,7 +6851,7 @@
         <v>0</v>
       </c>
       <c r="F153">
-        <v>36</v>
+        <v>88</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.35">
@@ -6887,7 +6871,7 @@
         <v>0</v>
       </c>
       <c r="F154">
-        <v>24</v>
+        <v>68</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.35">
@@ -6907,7 +6891,7 @@
         <v>0</v>
       </c>
       <c r="F155">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.35">
@@ -6927,7 +6911,7 @@
         <v>0</v>
       </c>
       <c r="F156">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.35">
@@ -6946,9 +6930,6 @@
       <c r="E157">
         <v>1</v>
       </c>
-      <c r="F157">
-        <v>12</v>
-      </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158">
@@ -6966,9 +6947,6 @@
       <c r="E158">
         <v>1</v>
       </c>
-      <c r="F158">
-        <v>8</v>
-      </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159">
@@ -6986,9 +6964,6 @@
       <c r="E159">
         <v>1</v>
       </c>
-      <c r="F159">
-        <v>11</v>
-      </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160">
@@ -7006,9 +6981,6 @@
       <c r="E160">
         <v>1</v>
       </c>
-      <c r="F160">
-        <v>68</v>
-      </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161">
@@ -7027,7 +6999,7 @@
         <v>0</v>
       </c>
       <c r="F161">
-        <v>24</v>
+        <v>68</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.35">
@@ -7047,7 +7019,7 @@
         <v>0</v>
       </c>
       <c r="F162">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.35">
@@ -7067,7 +7039,7 @@
         <v>0</v>
       </c>
       <c r="F163">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.35">
@@ -7086,6 +7058,9 @@
       <c r="E164">
         <v>0</v>
       </c>
+      <c r="F164">
+        <v>12</v>
+      </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165">
@@ -7103,6 +7078,9 @@
       <c r="E165">
         <v>0</v>
       </c>
+      <c r="F165">
+        <v>8</v>
+      </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166">
@@ -7120,6 +7098,9 @@
       <c r="E166">
         <v>0</v>
       </c>
+      <c r="F166">
+        <v>88</v>
+      </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167">
@@ -7154,6 +7135,9 @@
       <c r="E168">
         <v>0</v>
       </c>
+      <c r="F168">
+        <v>18</v>
+      </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169">
@@ -7171,6 +7155,9 @@
       <c r="E169">
         <v>0</v>
       </c>
+      <c r="F169">
+        <v>76</v>
+      </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170">
@@ -7188,6 +7175,9 @@
       <c r="E170">
         <v>0</v>
       </c>
+      <c r="F170">
+        <v>20</v>
+      </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171">
@@ -7205,6 +7195,9 @@
       <c r="E171">
         <v>0</v>
       </c>
+      <c r="F171">
+        <v>36</v>
+      </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172">
@@ -7222,6 +7215,9 @@
       <c r="E172">
         <v>0</v>
       </c>
+      <c r="F172">
+        <v>24</v>
+      </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173">
@@ -7239,6 +7235,9 @@
       <c r="E173">
         <v>0</v>
       </c>
+      <c r="F173">
+        <v>40</v>
+      </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174">
@@ -7273,6 +7272,9 @@
       <c r="E175">
         <v>0</v>
       </c>
+      <c r="F175">
+        <v>20</v>
+      </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176">
@@ -7290,8 +7292,11 @@
       <c r="E176">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F176">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>175</v>
       </c>
@@ -7307,8 +7312,11 @@
       <c r="E177">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F177">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>176</v>
       </c>
@@ -7324,8 +7332,11 @@
       <c r="E178">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F178">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>177</v>
       </c>
@@ -7341,8 +7352,11 @@
       <c r="E179">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F179">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>178</v>
       </c>
@@ -7358,8 +7372,11 @@
       <c r="E180">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F180">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>179</v>
       </c>
@@ -7375,8 +7392,11 @@
       <c r="E181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F181">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>180</v>
       </c>
@@ -7392,8 +7412,11 @@
       <c r="E182">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F182">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>181</v>
       </c>
@@ -7410,13 +7433,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E183" xr:uid="{59A9C8BC-438A-430A-B6C5-8193BB1DC93C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E183">
+  <autoFilter ref="A1:F183" xr:uid="{59A9C8BC-438A-430A-B6C5-8193BB1DC93C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F183">
       <sortCondition ref="A1:A183"/>
     </sortState>
   </autoFilter>

</xml_diff>